<commit_message>
archived old data when merging with dol
</commit_message>
<xml_diff>
--- a/excel_files/column_name_mappings.xlsx
+++ b/excel_files/column_name_mappings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexpiazza/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexpiazza/Desktop/for-db/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02967E14-526A-AE43-AD9E-C2D722C092C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDFD137-1F28-BD4C-9B0A-2615EC7C92B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{AF800995-AED1-F440-9025-2E69C06B710B}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{3D7FBC41-A7A1-3143-9EBD-1D76C3F8949B}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{3D7FBC41-A7A1-3143-9EBD-1D76C3F8949B}">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{B816DC5F-8D8A-D442-BFA2-62C7E6EDD424}">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{B816DC5F-8D8A-D442-BFA2-62C7E6EDD424}">
       <text>
         <r>
           <rPr>
@@ -110,7 +110,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="105">
   <si>
     <t>ETA case number</t>
   </si>
@@ -422,6 +422,9 @@
   </si>
   <si>
     <t>don't need that for DOL</t>
+  </si>
+  <si>
+    <t>column mappings to delete</t>
   </si>
 </sst>
 </file>
@@ -530,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -541,6 +544,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -855,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA62719-3303-4843-B6C0-235F8F677CDA}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -902,79 +906,79 @@
     </row>
     <row r="5" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>70</v>
@@ -982,233 +986,177 @@
     </row>
     <row r="15" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>76</v>
+        <v>44</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>74</v>
+        <v>41</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>77</v>
+        <v>45</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>78</v>
+        <v>43</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>79</v>
+        <v>42</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>81</v>
+        <v>48</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>82</v>
+        <v>49</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>83</v>
+        <v>50</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>84</v>
+        <v>51</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>85</v>
+        <v>52</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>86</v>
+        <v>53</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>87</v>
+        <v>54</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B43" s="6" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1220,15 +1168,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3ACA104-D856-444D-81F5-9A5317CB9A09}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="49" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -1320,37 +1269,99 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>94</v>
       </c>
     </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change column mappings for begin/end date
</commit_message>
<xml_diff>
--- a/excel_files/column_name_mappings.xlsx
+++ b/excel_files/column_name_mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexpiazza/Desktop/for-db/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDFD137-1F28-BD4C-9B0A-2615EC7C92B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96926226-9599-7A42-BD0F-50AC98C6C2FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{AF800995-AED1-F440-9025-2E69C06B710B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15780" xr2:uid="{AF800995-AED1-F440-9025-2E69C06B710B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,82 +33,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Microsoft Office User</author>
-  </authors>
-  <commentList>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{3D7FBC41-A7A1-3143-9EBD-1D76C3F8949B}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>also had EMPLOYMENT_BEGIN_DATA, but Lizzie email said to use the thing in yellow</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{B816DC5F-8D8A-D442-BFA2-62C7E6EDD424}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>also had EMPLOYMENT_END_DATE</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="105">
   <si>
@@ -172,12 +96,6 @@
     <t>Company zip code</t>
   </si>
   <si>
-    <t>REQUESTED_BEGIN_DATE</t>
-  </si>
-  <si>
-    <t>REQUESTED_END_DATE</t>
-  </si>
-  <si>
     <t>EMPLOYER_CITY</t>
   </si>
   <si>
@@ -425,13 +343,19 @@
   </si>
   <si>
     <t>column mappings to delete</t>
+  </si>
+  <si>
+    <t>EMPLOYMENT_BEGIN_DATE</t>
+  </si>
+  <si>
+    <t>EMPLOYMENT_END_DATE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -451,25 +375,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Menlo"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -495,18 +400,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -533,18 +432,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -858,11 +756,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA62719-3303-4843-B6C0-235F8F677CDA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA62719-3303-4843-B6C0-235F8F677CDA}">
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -924,16 +822,16 @@
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>20</v>
+      <c r="B7" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>21</v>
+      <c r="B8" s="6" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -941,7 +839,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -949,7 +847,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -957,172 +855,172 @@
         <v>19</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>81</v>
+        <v>42</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>82</v>
+        <v>39</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>83</v>
+        <v>43</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>84</v>
+        <v>41</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>85</v>
+        <v>40</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>77</v>
+        <v>49</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>78</v>
+        <v>50</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>10</v>
@@ -1130,39 +1028,38 @@
     </row>
     <row r="33" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>80</v>
+        <v>52</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1182,7 +1079,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1190,131 +1087,131 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
         <v>101</v>
-      </c>
-      <c r="B3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>10</v>
@@ -1322,18 +1219,18 @@
     </row>
     <row r="33" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -1346,18 +1243,18 @@
     </row>
     <row r="36" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>74</v>
+        <v>33</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enforces column datatypes, archives scraper data
</commit_message>
<xml_diff>
--- a/excel_files/column_name_mappings.xlsx
+++ b/excel_files/column_name_mappings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexpiazza/Desktop/for-db/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96926226-9599-7A42-BD0F-50AC98C6C2FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F9019F-5869-854C-99A1-CE42ACCDF67B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15780" xr2:uid="{AF800995-AED1-F440-9025-2E69C06B710B}"/>
   </bookViews>
@@ -75,9 +75,6 @@
     <t>WAGE_OFFER</t>
   </si>
   <si>
-    <t>Additional wage information</t>
-  </si>
-  <si>
     <t>FREQUENCY_OF_PAY</t>
   </si>
   <si>
@@ -349,6 +346,9 @@
   </si>
   <si>
     <t>EMPLOYMENT_END_DATE</t>
+  </si>
+  <si>
+    <t>Additional Wage Information</t>
   </si>
 </sst>
 </file>
@@ -760,7 +760,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -812,215 +812,215 @@
     </row>
     <row r="6" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>10</v>
@@ -1028,34 +1028,34 @@
     </row>
     <row r="33" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1079,7 +1079,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1087,131 +1087,131 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" t="s">
         <v>97</v>
-      </c>
-      <c r="B13" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>10</v>
@@ -1219,18 +1219,18 @@
     </row>
     <row r="33" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -1243,18 +1243,18 @@
     </row>
     <row r="36" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>